<commit_message>
Add loss functions and use different layers no. Add more data to the original dataset.
</commit_message>
<xml_diff>
--- a/fake_news_impl/datasets/set3.xlsx
+++ b/fake_news_impl/datasets/set3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="23325" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="127">
   <si>
     <t>source:</t>
   </si>
@@ -294,9 +294,6 @@
     <t>In 1996, when Nigeria was hit by meningitis epidemic, a hundred children were given an experimental oral antibiotic Trovan developed by Pfizer, while a further hundred received ceftriaxone, the â€œgold-standardâ€ treatment of modern medicine. Five children died after taking Trovan and six â€“ after taking ceftriaxone. But later it was claimed that Pfizer did not have proper consent from parents to use an experimental drug on their children and questions were raised over the documentation of the trial. Legal action filed against the company alleged that some received a dose lower than recommended, leaving many children with brain damage, paralysis or slurred speech. Pfizer had argued that meningitis and not its antibiotic had led to the deaths of 11 children. Ultimately, following a 15-year court dispute, Pfizer paid out USD 175,000 to the families of four of the children each.</t>
   </si>
   <si>
-    <t>Partially false</t>
-  </si>
-  <si>
     <t>In 1996 Pfizer tested an experimental antibiotic (Trovan) in parallel to ceftriaxone (gold standard) on a hundred minors each in Nigeria, and there were reported five deaths in the Trovan group and six in the cefrtiaxone one, not "two hundred deaths". The parents' informed consent and the suitability of the dosage (allegedly too low) has been called into question and after a 15-year court dispute, Pfizer paid out USD 175,000 to the families of four of the children each.</t>
   </si>
   <si>
@@ -397,19 +394,16 @@
   </si>
   <si>
     <t>The claim that clinical trials in Indonesia recorded Sinovac's COVID-19 vaccine as having a 91.25% efficacy rate is false, the efficacy rate in Indonesia is 65.3% and in Turkey is 91.25% for Phase III trials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,331 +419,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -757,232 +436,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1273,27 +743,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="106.285714285714" customWidth="1"/>
-    <col min="3" max="3" width="136.142857142857" customWidth="1"/>
+    <col min="2" max="2" width="106.28515625" customWidth="1"/>
+    <col min="3" max="3" width="136.140625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="255.714285714286" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>81</v>
       </c>
@@ -1328,11 +798,8 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>82</v>
       </c>
@@ -1345,11 +812,8 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>83</v>
       </c>
@@ -1362,11 +826,8 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>84</v>
       </c>
@@ -1379,11 +840,8 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>85</v>
       </c>
@@ -1396,11 +854,8 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>86</v>
       </c>
@@ -1413,11 +868,8 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>87</v>
       </c>
@@ -1430,11 +882,8 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>88</v>
       </c>
@@ -1447,11 +896,8 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>89</v>
       </c>
@@ -1464,11 +910,8 @@
       <c r="D12" t="b">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>90</v>
       </c>
@@ -1481,11 +924,8 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>91</v>
       </c>
@@ -1498,11 +938,8 @@
       <c r="D14" t="b">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>92</v>
       </c>
@@ -1515,11 +952,8 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>93</v>
       </c>
@@ -1532,11 +966,8 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>94</v>
       </c>
@@ -1549,11 +980,8 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>95</v>
       </c>
@@ -1566,11 +994,8 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>96</v>
       </c>
@@ -1583,11 +1008,8 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>97</v>
       </c>
@@ -1600,11 +1022,8 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>98</v>
       </c>
@@ -1617,11 +1036,8 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>99</v>
       </c>
@@ -1634,11 +1050,8 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>100</v>
       </c>
@@ -1651,11 +1064,8 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>101</v>
       </c>
@@ -1668,11 +1078,8 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>102</v>
       </c>
@@ -1685,11 +1092,8 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>103</v>
       </c>
@@ -1702,11 +1106,8 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>104</v>
       </c>
@@ -1719,11 +1120,8 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
-      <c r="E27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>105</v>
       </c>
@@ -1736,11 +1134,8 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>106</v>
       </c>
@@ -1753,11 +1148,8 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>107</v>
       </c>
@@ -1770,11 +1162,8 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>108</v>
       </c>
@@ -1787,11 +1176,8 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
-      <c r="E31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>109</v>
       </c>
@@ -1801,237 +1187,752 @@
       <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="D32" t="s">
-        <v>92</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>110</v>
       </c>
       <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
-        <v>95</v>
-      </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
-      <c r="E33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>111</v>
       </c>
       <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
-      <c r="E34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>112</v>
       </c>
       <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
-        <v>101</v>
-      </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
-      <c r="E35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>113</v>
       </c>
       <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
-      <c r="E36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>114</v>
       </c>
       <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
         <v>106</v>
       </c>
-      <c r="C37" t="s">
-        <v>107</v>
-      </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
-      <c r="E37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>115</v>
       </c>
       <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
         <v>109</v>
       </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>116</v>
       </c>
       <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="C39" t="s">
-        <v>113</v>
-      </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
-      <c r="E39" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>117</v>
       </c>
       <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
-        <v>116</v>
-      </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
-      <c r="E40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>118</v>
       </c>
       <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
         <v>118</v>
       </c>
-      <c r="C41" t="s">
-        <v>119</v>
-      </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
-      <c r="E41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>119</v>
       </c>
       <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
         <v>121</v>
       </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
-      <c r="E42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>120</v>
       </c>
       <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
         <v>124</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>121</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>122</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>123</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>124</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
         <v>125</v>
       </c>
-      <c r="D43" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
         <v>126</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>128</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>129</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>130</v>
+      </c>
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>131</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>134</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>135</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>136</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>137</v>
+      </c>
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>138</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>139</v>
+      </c>
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>140</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>141</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>142</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>143</v>
+      </c>
+      <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>144</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>146</v>
+      </c>
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>147</v>
+      </c>
+      <c r="B70" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>148</v>
+      </c>
+      <c r="B71" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>149</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>150</v>
+      </c>
+      <c r="B73" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>151</v>
+      </c>
+      <c r="B74" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>152</v>
+      </c>
+      <c r="B75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>153</v>
+      </c>
+      <c r="B76" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>155</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" t="s">
+        <v>112</v>
+      </c>
+      <c r="D79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" t="s">
+        <v>115</v>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
+      </c>
+      <c r="D81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>159</v>
+      </c>
+      <c r="B82" t="s">
+        <v>122</v>
+      </c>
+      <c r="C82" t="s">
+        <v>121</v>
+      </c>
+      <c r="D82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>160</v>
+      </c>
+      <c r="B83" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://www.poynter.org/ifcn-covid-19-misinformation/?covid_countries=0&amp;covid_rating=51174&amp;covid_fact_checkers=0"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>